<commit_message>
changed all IMU values to be stored in typdef struct instead of random globals all over. Much more organized now. next, validate the rotate_to_world() function and calibrate the LIDAR sensor
</commit_message>
<xml_diff>
--- a/BNO055_calib_test_result.xlsx
+++ b/BNO055_calib_test_result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mak/Documents/PlatformIO/Projects/bnolqr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9BE7D5E4-D190-E84E-839A-93A385F8DC44}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC15384-81F3-DB4E-A4AE-DFDCA8D5E864}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="78680" yWindow="8380" windowWidth="27240" windowHeight="16440" xr2:uid="{7D137BA7-906B-D24B-92B4-0B2DDB3FB37D}"/>
   </bookViews>
@@ -371,15 +371,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A08B13-DDA1-C045-B97A-A596957A8500}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>51</v>
       </c>
@@ -398,8 +398,11 @@
       <c r="F1">
         <v>-20</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-179</v>
       </c>
@@ -418,8 +421,11 @@
       <c r="F2">
         <v>-176</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>-176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>-19</v>
       </c>
@@ -438,8 +444,11 @@
       <c r="F3">
         <v>-30</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>6519</v>
       </c>
@@ -458,8 +467,11 @@
       <c r="F5">
         <v>6472</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>6472</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>-2144</v>
       </c>
@@ -478,8 +490,11 @@
       <c r="F6">
         <v>-2144</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>-2144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>732</v>
       </c>
@@ -498,8 +513,11 @@
       <c r="F7">
         <v>731</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>-1</v>
       </c>
@@ -518,8 +536,11 @@
       <c r="F9">
         <v>-1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -538,8 +559,11 @@
       <c r="F10">
         <v>-1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>-1</v>
       </c>
@@ -558,8 +582,11 @@
       <c r="F11">
         <v>-1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1000</v>
       </c>
@@ -570,7 +597,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>776</v>
       </c>
@@ -579,6 +606,42 @@
       </c>
       <c r="C14">
         <v>776</v>
+      </c>
+    </row>
+    <row r="19" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I19">
+        <f>AVERAGE(B1:O1)</f>
+        <v>-21.5</v>
+      </c>
+    </row>
+    <row r="20" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I20">
+        <f>AVERAGE(A2:O2)</f>
+        <v>-176.71428571428572</v>
+      </c>
+    </row>
+    <row r="21" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I21">
+        <f>AVERAGE(C3:R3)</f>
+        <v>-32.6</v>
+      </c>
+    </row>
+    <row r="23" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I23">
+        <f>AVERAGE(A5:P5)</f>
+        <v>6465.8571428571431</v>
+      </c>
+    </row>
+    <row r="24" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I24">
+        <f>AVERAGE(A6:R6)</f>
+        <v>-2144.8571428571427</v>
+      </c>
+    </row>
+    <row r="25" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I25">
+        <f>AVERAGE(A7:P7)</f>
+        <v>724.85714285714289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>